<commit_message>
bug when inputting data fixed
</commit_message>
<xml_diff>
--- a/testingBook.xlsx
+++ b/testingBook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcao2\PycharmProjects\EVStation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD9BA54-E264-40CE-AB08-3849C0569EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2F836F-A24B-4280-B7E1-FBC84C6F6AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05.22" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="24">
   <si>
     <t>Driver Name</t>
   </si>
@@ -1472,8 +1472,8 @@
     <col min="7" max="7" width="11.81640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.6328125" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.36328125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="8.36328125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.36328125" style="1"/>
+    <col min="10" max="13" width="8.36328125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.36328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" customHeight="1">
@@ -1911,7 +1911,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="37.5">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.5">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>161.62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="37.5">
+    <row r="3" spans="1:9" ht="37.5" customHeight="1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>102.74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="37.5">
+    <row r="4" spans="1:9" ht="37.5" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>14.46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" customHeight="1">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="37.5">
+    <row r="6" spans="1:9" ht="37.5" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5">
+    <row r="7" spans="1:9" ht="37.5" customHeight="1">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>102.83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.5">
+    <row r="8" spans="1:9" ht="37.5" customHeight="1">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="37.5">
+    <row r="9" spans="1:9" ht="37.5" customHeight="1">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>94.48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="37.5">
+    <row r="10" spans="1:9" ht="37.5" customHeight="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="37.5">
+    <row r="11" spans="1:9" ht="37.5" customHeight="1">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="37.5">
+    <row r="12" spans="1:9" ht="37.5" customHeight="1">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>240.32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.5">
+    <row r="13" spans="1:9" ht="37.5" customHeight="1">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>91.54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.5">
+    <row r="14" spans="1:9" ht="37.5" customHeight="1">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="37.5">
+    <row r="15" spans="1:9" ht="37.5" customHeight="1">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2317,7 +2317,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="37.5">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.5">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>161.62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="37.5">
+    <row r="3" spans="1:9" ht="37.5" customHeight="1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>102.74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="37.5">
+    <row r="4" spans="1:9" ht="37.5" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>14.46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" customHeight="1">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="37.5">
+    <row r="6" spans="1:9" ht="37.5" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5">
+    <row r="7" spans="1:9" ht="37.5" customHeight="1">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>102.83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.5">
+    <row r="8" spans="1:9" ht="37.5" customHeight="1">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="37.5">
+    <row r="9" spans="1:9" ht="37.5" customHeight="1">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>94.48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="37.5">
+    <row r="10" spans="1:9" ht="37.5" customHeight="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="37.5">
+    <row r="11" spans="1:9" ht="37.5" customHeight="1">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="37.5">
+    <row r="12" spans="1:9" ht="37.5" customHeight="1">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>240.32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.5">
+    <row r="13" spans="1:9" ht="37.5" customHeight="1">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>91.54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.5">
+    <row r="14" spans="1:9" ht="37.5" customHeight="1">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="37.5">
+    <row r="15" spans="1:9" ht="37.5" customHeight="1">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2723,7 +2723,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="37.5">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.5">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>161.62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="37.5">
+    <row r="3" spans="1:9" ht="37.5" customHeight="1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>102.74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="37.5">
+    <row r="4" spans="1:9" ht="37.5" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>14.46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" customHeight="1">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="37.5">
+    <row r="6" spans="1:9" ht="37.5" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5">
+    <row r="7" spans="1:9" ht="37.5" customHeight="1">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>102.83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.5">
+    <row r="8" spans="1:9" ht="37.5" customHeight="1">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="37.5">
+    <row r="9" spans="1:9" ht="37.5" customHeight="1">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>94.48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="37.5">
+    <row r="10" spans="1:9" ht="37.5" customHeight="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="37.5">
+    <row r="11" spans="1:9" ht="37.5" customHeight="1">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="37.5">
+    <row r="12" spans="1:9" ht="37.5" customHeight="1">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>240.32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.5">
+    <row r="13" spans="1:9" ht="37.5" customHeight="1">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>91.54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.5">
+    <row r="14" spans="1:9" ht="37.5" customHeight="1">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="37.5">
+    <row r="15" spans="1:9" ht="37.5" customHeight="1">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -3129,7 +3129,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="37.5">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.5">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>161.62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="37.5">
+    <row r="3" spans="1:9" ht="37.5" customHeight="1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>102.74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="37.5">
+    <row r="4" spans="1:9" ht="37.5" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>14.46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" customHeight="1">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="37.5">
+    <row r="6" spans="1:9" ht="37.5" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5">
+    <row r="7" spans="1:9" ht="37.5" customHeight="1">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>102.83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.5">
+    <row r="8" spans="1:9" ht="37.5" customHeight="1">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="37.5">
+    <row r="9" spans="1:9" ht="37.5" customHeight="1">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>94.48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="37.5">
+    <row r="10" spans="1:9" ht="37.5" customHeight="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="37.5">
+    <row r="11" spans="1:9" ht="37.5" customHeight="1">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="37.5">
+    <row r="12" spans="1:9" ht="37.5" customHeight="1">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>240.32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.5">
+    <row r="13" spans="1:9" ht="37.5" customHeight="1">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>91.54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.5">
+    <row r="14" spans="1:9" ht="37.5" customHeight="1">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="37.5">
+    <row r="15" spans="1:9" ht="37.5" customHeight="1">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -3529,12 +3529,408 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="37.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="37.5">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>134</v>
+      </c>
+      <c r="D2">
+        <v>855.89700000000005</v>
+      </c>
+      <c r="E2">
+        <v>607.68700000000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>0.18</v>
+      </c>
+      <c r="H2">
+        <v>9.56</v>
+      </c>
+      <c r="I2">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="37.5">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>569.14599999999996</v>
+      </c>
+      <c r="E3">
+        <v>404.09300000000002</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>3.83</v>
+      </c>
+      <c r="H3">
+        <v>11.09</v>
+      </c>
+      <c r="I3">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="37.5">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>72.287000000000006</v>
+      </c>
+      <c r="E4">
+        <v>51.323999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>14.46</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>14.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="37.5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>61.372999999999998</v>
+      </c>
+      <c r="E5">
+        <v>43.575000000000003</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>12.27</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5">
+        <v>12.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="37.5">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>375.00700000000001</v>
+      </c>
+      <c r="E6">
+        <v>266.255</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>75</v>
+      </c>
+      <c r="H6">
+        <v>5.2</v>
+      </c>
+      <c r="I6">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="37.5">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>558.38199999999995</v>
+      </c>
+      <c r="E7">
+        <v>396.45100000000002</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>111.68</v>
+      </c>
+      <c r="H7">
+        <v>8.85</v>
+      </c>
+      <c r="I7">
+        <v>102.83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="37.5">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>75</v>
+      </c>
+      <c r="D8">
+        <v>473.78699999999998</v>
+      </c>
+      <c r="E8">
+        <v>336.38799999999998</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>94.76</v>
+      </c>
+      <c r="H8">
+        <v>0.01</v>
+      </c>
+      <c r="I8">
+        <v>94.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="37.5">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>478.07900000000001</v>
+      </c>
+      <c r="E9">
+        <v>339.43599999999998</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>95.62</v>
+      </c>
+      <c r="H9">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I9">
+        <v>94.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="37.5">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="37.5">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>266.33999999999997</v>
+      </c>
+      <c r="E11">
+        <v>189.101</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>53.27</v>
+      </c>
+      <c r="H11">
+        <v>42.97</v>
+      </c>
+      <c r="I11">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="37.5">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>81</v>
+      </c>
+      <c r="D12">
+        <v>1250.682</v>
+      </c>
+      <c r="E12">
+        <v>887.98400000000004</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>250.14</v>
+      </c>
+      <c r="H12">
+        <v>9.82</v>
+      </c>
+      <c r="I12">
+        <v>240.32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="37.5">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>52</v>
+      </c>
+      <c r="D13">
+        <v>1108.7149999999999</v>
+      </c>
+      <c r="E13">
+        <v>787.18799999999999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>221.74</v>
+      </c>
+      <c r="H13">
+        <v>130.19999999999999</v>
+      </c>
+      <c r="I13">
+        <v>91.54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="37.5">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>135.28200000000001</v>
+      </c>
+      <c r="E14">
+        <v>96.051000000000002</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>27.06</v>
+      </c>
+      <c r="H14">
+        <v>21.77</v>
+      </c>
+      <c r="I14">
+        <v>5.29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="37.5">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>51.466999999999999</v>
+      </c>
+      <c r="E15">
+        <v>36.542000000000002</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>10.29</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>10.29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3555,13 +3951,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="37.5">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3590,7 +3986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.5">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3616,7 +4012,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="37.5">
+    <row r="3" spans="1:9" ht="37.5" customHeight="1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3642,7 +4038,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="37.5">
+    <row r="4" spans="1:9" ht="37.5" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3668,7 +4064,7 @@
         <v>4.46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" customHeight="1">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3694,7 +4090,7 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="37.5">
+    <row r="6" spans="1:9" ht="37.5" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3720,7 +4116,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5">
+    <row r="7" spans="1:9" ht="37.5" customHeight="1">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3746,7 +4142,7 @@
         <v>102.83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.5">
+    <row r="8" spans="1:9" ht="37.5" customHeight="1">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -3772,7 +4168,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="37.5">
+    <row r="9" spans="1:9" ht="37.5" customHeight="1">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3798,7 +4194,7 @@
         <v>94.48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="37.5">
+    <row r="10" spans="1:9" ht="37.5" customHeight="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3824,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="37.5">
+    <row r="11" spans="1:9" ht="37.5" customHeight="1">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3850,7 +4246,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="37.5">
+    <row r="12" spans="1:9" ht="37.5" customHeight="1">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3876,7 +4272,7 @@
         <v>20.32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.5">
+    <row r="13" spans="1:9" ht="37.5" customHeight="1">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3902,7 +4298,7 @@
         <v>91.54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.5">
+    <row r="14" spans="1:9" ht="37.5" customHeight="1">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3928,7 +4324,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="37.5">
+    <row r="15" spans="1:9" ht="37.5" customHeight="1">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -3969,7 +4365,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="37.5">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3998,7 +4394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.5">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4024,7 +4420,7 @@
         <v>11.62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="37.5">
+    <row r="3" spans="1:9" ht="37.5" customHeight="1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4050,7 +4446,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="37.5">
+    <row r="4" spans="1:9" ht="37.5" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4076,7 +4472,7 @@
         <v>14.46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" customHeight="1">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -4102,7 +4498,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="37.5">
+    <row r="6" spans="1:9" ht="37.5" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -4128,7 +4524,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5">
+    <row r="7" spans="1:9" ht="37.5" customHeight="1">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4154,7 +4550,7 @@
         <v>102.83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="37.5">
+    <row r="8" spans="1:9" ht="37.5" customHeight="1">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -4180,7 +4576,7 @@
         <v>94.75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="37.5">
+    <row r="9" spans="1:9" ht="37.5" customHeight="1">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4206,7 +4602,7 @@
         <v>94.48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="37.5">
+    <row r="10" spans="1:9" ht="37.5" customHeight="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4232,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="37.5">
+    <row r="11" spans="1:9" ht="37.5" customHeight="1">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -4258,7 +4654,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="37.5">
+    <row r="12" spans="1:9" ht="37.5" customHeight="1">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -4284,7 +4680,7 @@
         <v>240.32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.5">
+    <row r="13" spans="1:9" ht="37.5" customHeight="1">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -4310,7 +4706,7 @@
         <v>91.54</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.5">
+    <row r="14" spans="1:9" ht="37.5" customHeight="1">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -4336,7 +4732,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="37.5">
+    <row r="15" spans="1:9" ht="37.5" customHeight="1">
       <c r="A15" t="s">
         <v>23</v>
       </c>

</xml_diff>